<commit_message>
Adds some commands to the documentation
</commit_message>
<xml_diff>
--- a/doc/Spec.xlsx
+++ b/doc/Spec.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Sequence</t>
   </si>
@@ -105,6 +105,18 @@
   </si>
   <si>
     <t xml:space="preserve">Packets/Second </t>
+  </si>
+  <si>
+    <t>BUFF_LOAD</t>
+  </si>
+  <si>
+    <t>SHOW_MODE</t>
+  </si>
+  <si>
+    <t>Tells the micro to start looking for packets</t>
+  </si>
+  <si>
+    <t>Tells the mirco to just light up drums that were hit</t>
   </si>
 </sst>
 </file>
@@ -328,6 +340,11 @@
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -337,11 +354,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -636,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:B18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,433 +661,441 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="9"/>
+      <c r="D1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="2">
         <v>31</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="2">
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="2">
         <v>30</v>
       </c>
       <c r="B4" s="11"/>
-      <c r="D4" s="5">
+      <c r="D4" s="2">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="2">
         <v>29</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="2">
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="2">
         <v>28</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="D6" s="5">
+      <c r="D6" s="2">
         <v>3</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="2">
         <v>27</v>
       </c>
       <c r="B7" s="12"/>
-      <c r="D7" s="5">
+      <c r="D7" s="2">
         <v>4</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="2">
         <v>26</v>
       </c>
       <c r="B8" s="12"/>
-      <c r="D8" s="5">
+      <c r="D8" s="2">
         <v>5</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="2">
         <v>25</v>
       </c>
       <c r="B9" s="12"/>
-      <c r="D9" s="5">
+      <c r="D9" s="2">
         <v>6</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="2">
         <v>24</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="D10" s="5">
+      <c r="D10" s="2">
         <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="2">
         <v>23</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="2">
         <v>8</v>
       </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="6"/>
+      <c r="E11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+      <c r="A12" s="2">
         <v>22</v>
       </c>
       <c r="B12" s="12"/>
-      <c r="D12" s="5">
+      <c r="D12" s="2">
         <v>9</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="6"/>
+      <c r="E12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+      <c r="A13" s="2">
         <v>21</v>
       </c>
       <c r="B13" s="12"/>
-      <c r="D13" s="5">
+      <c r="D13" s="2">
         <v>10</v>
       </c>
       <c r="E13" s="1"/>
-      <c r="F13" s="6"/>
+      <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="A14" s="2">
         <v>20</v>
       </c>
       <c r="B14" s="12"/>
-      <c r="D14" s="5">
+      <c r="D14" s="2">
         <v>11</v>
       </c>
       <c r="E14" s="1"/>
-      <c r="F14" s="6"/>
+      <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+      <c r="A15" s="2">
         <v>19</v>
       </c>
       <c r="B15" s="12"/>
-      <c r="D15" s="5">
+      <c r="D15" s="2">
         <v>12</v>
       </c>
       <c r="E15" s="1"/>
-      <c r="F15" s="6"/>
+      <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="A16" s="2">
         <v>18</v>
       </c>
       <c r="B16" s="12"/>
-      <c r="D16" s="5">
+      <c r="D16" s="2">
         <v>13</v>
       </c>
       <c r="E16" s="1"/>
-      <c r="F16" s="6"/>
+      <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+      <c r="A17" s="2">
         <v>17</v>
       </c>
       <c r="B17" s="12"/>
-      <c r="D17" s="5">
+      <c r="D17" s="2">
         <v>14</v>
       </c>
       <c r="E17" s="1"/>
-      <c r="F17" s="6"/>
+      <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+      <c r="A18" s="2">
         <v>16</v>
       </c>
       <c r="B18" s="11"/>
-      <c r="D18" s="5">
+      <c r="D18" s="2">
         <v>15</v>
       </c>
       <c r="E18" s="1"/>
-      <c r="F18" s="6"/>
+      <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
+      <c r="A19" s="2">
         <v>15</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="2">
         <v>16</v>
       </c>
       <c r="E19" s="1"/>
-      <c r="F19" s="6"/>
+      <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
+      <c r="A20" s="2">
         <v>14</v>
       </c>
       <c r="B20" s="12"/>
-      <c r="D20" s="5">
+      <c r="D20" s="2">
         <v>17</v>
       </c>
       <c r="E20" s="1"/>
-      <c r="F20" s="6"/>
+      <c r="F20" s="3"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
+      <c r="A21" s="2">
         <v>13</v>
       </c>
       <c r="B21" s="12"/>
-      <c r="D21" s="5">
+      <c r="D21" s="2">
         <v>18</v>
       </c>
       <c r="E21" s="1"/>
-      <c r="F21" s="6"/>
+      <c r="F21" s="3"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
+      <c r="A22" s="2">
         <v>12</v>
       </c>
       <c r="B22" s="12"/>
-      <c r="D22" s="5">
+      <c r="D22" s="2">
         <v>19</v>
       </c>
       <c r="E22" s="1"/>
-      <c r="F22" s="6"/>
+      <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
+      <c r="A23" s="2">
         <v>11</v>
       </c>
       <c r="B23" s="12"/>
-      <c r="D23" s="5">
+      <c r="D23" s="2">
         <v>20</v>
       </c>
       <c r="E23" s="1"/>
-      <c r="F23" s="6"/>
+      <c r="F23" s="3"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
+      <c r="A24" s="2">
         <v>10</v>
       </c>
       <c r="B24" s="12"/>
-      <c r="D24" s="5">
+      <c r="D24" s="2">
         <v>21</v>
       </c>
       <c r="E24" s="1"/>
-      <c r="F24" s="6"/>
+      <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
+      <c r="A25" s="2">
         <v>9</v>
       </c>
       <c r="B25" s="12"/>
-      <c r="D25" s="5">
+      <c r="D25" s="2">
         <v>22</v>
       </c>
       <c r="E25" s="1"/>
-      <c r="F25" s="6"/>
+      <c r="F25" s="3"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
+      <c r="A26" s="2">
         <v>8</v>
       </c>
       <c r="B26" s="12"/>
-      <c r="D26" s="5">
+      <c r="D26" s="2">
         <v>23</v>
       </c>
       <c r="E26" s="1"/>
-      <c r="F26" s="6"/>
+      <c r="F26" s="3"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
+      <c r="A27" s="2">
         <v>7</v>
       </c>
       <c r="B27" s="12"/>
-      <c r="D27" s="5">
+      <c r="D27" s="2">
         <v>24</v>
       </c>
       <c r="E27" s="1"/>
-      <c r="F27" s="6"/>
+      <c r="F27" s="3"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
+      <c r="A28" s="2">
         <v>6</v>
       </c>
       <c r="B28" s="12"/>
-      <c r="D28" s="5">
+      <c r="D28" s="2">
         <v>25</v>
       </c>
       <c r="E28" s="1"/>
-      <c r="F28" s="6"/>
+      <c r="F28" s="3"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
+      <c r="A29" s="2">
         <v>5</v>
       </c>
       <c r="B29" s="12"/>
-      <c r="D29" s="5">
+      <c r="D29" s="2">
         <v>26</v>
       </c>
       <c r="E29" s="1"/>
-      <c r="F29" s="6"/>
+      <c r="F29" s="3"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
+      <c r="A30" s="2">
         <v>4</v>
       </c>
       <c r="B30" s="12"/>
-      <c r="D30" s="5">
+      <c r="D30" s="2">
         <v>27</v>
       </c>
       <c r="E30" s="1"/>
-      <c r="F30" s="6"/>
+      <c r="F30" s="3"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="5">
+      <c r="A31" s="2">
         <v>3</v>
       </c>
       <c r="B31" s="12"/>
-      <c r="D31" s="5">
+      <c r="D31" s="2">
         <v>28</v>
       </c>
       <c r="E31" s="1"/>
-      <c r="F31" s="6"/>
+      <c r="F31" s="3"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="5">
+      <c r="A32" s="2">
         <v>2</v>
       </c>
       <c r="B32" s="12"/>
-      <c r="D32" s="5">
+      <c r="D32" s="2">
         <v>29</v>
       </c>
       <c r="E32" s="1"/>
-      <c r="F32" s="6"/>
+      <c r="F32" s="3"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="5">
+      <c r="A33" s="2">
         <v>1</v>
       </c>
       <c r="B33" s="12"/>
-      <c r="D33" s="5">
+      <c r="D33" s="2">
         <v>30</v>
       </c>
       <c r="E33" s="1"/>
-      <c r="F33" s="6"/>
+      <c r="F33" s="3"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="7">
+      <c r="A34" s="4">
         <v>0</v>
       </c>
       <c r="B34" s="13"/>
-      <c r="D34" s="7">
+      <c r="D34" s="4">
         <v>31</v>
       </c>
-      <c r="E34" s="8"/>
-      <c r="F34" s="9"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B19:B34"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B10"/>
     <mergeCell ref="B11:B18"/>
-    <mergeCell ref="B19:B34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>